<commit_message>
Added Python and MySQL cheatsheet
</commit_message>
<xml_diff>
--- a/SQL Cheatsheet.xlsx
+++ b/SQL Cheatsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE14762E-552C-4B95-A6AE-223243269782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB811277-73D3-4444-A32B-8CD220077C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E4A5F62C-8D06-41C7-B4DE-EB3603C85B7B}"/>
+    <workbookView xWindow="28680" yWindow="5895" windowWidth="29040" windowHeight="15720" xr2:uid="{E4A5F62C-8D06-41C7-B4DE-EB3603C85B7B}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL Basics" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Concept</t>
   </si>
@@ -1484,6 +1484,191 @@
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Choose from only a select number of items when creating the table with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ENUM</t>
+    </r>
+  </si>
+  <si>
+    <t>Automatically auto-increment the Primary Key and add NOT NULL</t>
+  </si>
+  <si>
+    <t>Set a default value for columns in a table</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE TABLE Person(
+    personID INT PRIMARY KEY NOT NULL </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AUTO_INCREMENT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+    name VARCHAR(50) NOT NULL,
+    gender ENUM('M', 'F', 'O') NOT NULL,
+);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE TABLE Person(
+    personID INT PRIMARY KEY,
+    name VARCHAR(50),
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> gender ENUM('M', 'F', 'O'),</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CREATE TABLE Score(
+    scoreID INT PRIMARY KEY NOT NULL AUTO_INCREMENT,
+    score1 INT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEFAULT 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,
+    score2 INT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEFAULT 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We can create default values with the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEFAULT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> keyword, then insert whatever we'd like afterwards.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AUTO_INCREMENT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> keyword makes it so that we don't need to manually insert the primary key all the time</t>
     </r>
   </si>
 </sst>
@@ -1675,8 +1860,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F6ADFDBF-32B0-4AE5-8A41-A09672AA5465}" name="Table1" displayName="Table1" ref="A1:E26" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E26" xr:uid="{F6ADFDBF-32B0-4AE5-8A41-A09672AA5465}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F6ADFDBF-32B0-4AE5-8A41-A09672AA5465}" name="Table1" displayName="Table1" ref="A1:E29" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E29" xr:uid="{F6ADFDBF-32B0-4AE5-8A41-A09672AA5465}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DBC7B815-F2A7-4DA5-8441-47B7F550B802}" name="Concept" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{ED6369AD-69D7-4F5F-B95F-CDD4EC63D99D}" name="Code" dataDxfId="3"/>
@@ -1985,15 +2170,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F752F51-D0E3-4E26-9966-8896CF2092BE}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="78.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
@@ -2038,7 +2223,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -2046,7 +2231,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2146,7 +2331,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -2196,7 +2381,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
@@ -2224,7 +2409,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -2246,7 +2431,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -2257,7 +2442,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -2282,7 +2467,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>73</v>
       </c>
@@ -2313,7 +2498,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
@@ -2322,6 +2507,36 @@
       </c>
       <c r="C26" s="1" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Cheatsheets for Kent Uni
</commit_message>
<xml_diff>
--- a/SQL Cheatsheet.xlsx
+++ b/SQL Cheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB811277-73D3-4444-A32B-8CD220077C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24E25FE-5747-4985-A584-EF2D5D0E19D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="5895" windowWidth="29040" windowHeight="15720" xr2:uid="{E4A5F62C-8D06-41C7-B4DE-EB3603C85B7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E4A5F62C-8D06-41C7-B4DE-EB3603C85B7B}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL Basics" sheetId="1" r:id="rId1"/>
@@ -2172,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F752F51-D0E3-4E26-9966-8896CF2092BE}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>